<commit_message>
Subida con el 66% Noviembre
</commit_message>
<xml_diff>
--- a/Datos/DatosOficiales/BDTESISCOEF.xlsx
+++ b/Datos/DatosOficiales/BDTESISCOEF.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\Tesis\Datos\DatosOficiales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F336B1-6F47-4923-9ED2-EC7AE32CD195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22DE1FA-0753-4F2D-AA4F-D75079AF9021}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6525" yWindow="6525" windowWidth="22095" windowHeight="8340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$J$109</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -485,7 +488,7 @@
   <dimension ref="A1:J208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M119" sqref="M119"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5077,6 +5080,7 @@
       <c r="I208" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J109" xr:uid="{0713E84F-3633-4DFB-BC6E-8CDD0CEC9906}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>